<commit_message>
some scripting and data stuff
Co-authored-by: Magnus K. Lundgren <magnusklundgren@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/outputs/answer_labels/mintaka_dev_answer_labels_sheet.xlsx
+++ b/outputs/answer_labels/mintaka_dev_answer_labels_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lasse\Documents\6sem\Project\dataset-generation\outputs\answer_labels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F314E7F-FF6F-4F71-8C60-D4E485991F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AFA3EC-23E1-4251-83B7-592E9DFCF5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15558,7 +15558,7 @@
   <dimension ref="A1:G1575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>